<commit_message>
Update unit test for the new MSTemplate_Creator.
</commit_message>
<xml_diff>
--- a/tests/testdata/test_sample_annot/WideTableForm_Annotation_WithMissingSamples.xlsx
+++ b/tests/testdata/test_sample_annot/WideTableForm_Annotation_WithMissingSamples.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MSOrganiser\tests\testdata\test_sample_annot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94C0ABA0-E9F8-4D3B-9DCC-AD6B7B8A4F4D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31A743A1-8ED6-4B18-AD2F-019AC7602368}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16770" windowHeight="8775" activeTab="2" xr2:uid="{99D2A2AC-8431-4E91-B3F6-6736E2B6E0B0}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16770" windowHeight="8775" xr2:uid="{99D2A2AC-8431-4E91-B3F6-6736E2B6E0B0}"/>
   </bookViews>
   <sheets>
     <sheet name="Transition_Name_Annot" sheetId="1" r:id="rId1"/>
@@ -77,9 +77,6 @@
     <t>to</t>
   </si>
   <si>
-    <t>[uM] or [nmol/mL]</t>
-  </si>
-  <si>
     <t>Data_File_Name</t>
   </si>
   <si>
@@ -240,6 +237,9 @@
   </si>
   <si>
     <t>48_PQC_17</t>
+  </si>
+  <si>
+    <t>[uM] or [pmol/uL]</t>
   </si>
 </sst>
 </file>
@@ -592,7 +592,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4803233F-B712-4161-B593-AE755CB87014}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -673,9 +673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0EE0EDE-6E6E-44DD-9406-BA9457E2E392}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -683,6 +681,7 @@
     <col min="2" max="2" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -715,7 +714,7 @@
         <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -761,7 +760,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71DDAA14-6FD5-4E8E-8E4E-5626FCBDE549}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -777,1042 +776,1042 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>18</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>20</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>21</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>22</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>23</v>
-      </c>
-      <c r="H1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
         <v>26</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" t="s">
-        <v>28</v>
-      </c>
       <c r="E2">
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G2">
         <v>190</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3">
         <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G3">
         <v>190</v>
       </c>
       <c r="H3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4">
         <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G4">
         <v>190</v>
       </c>
       <c r="H4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5">
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G5">
         <v>190</v>
       </c>
       <c r="H5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6">
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G6">
         <v>190</v>
       </c>
       <c r="H6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7">
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G7">
         <v>190</v>
       </c>
       <c r="H7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
         <v>36</v>
       </c>
-      <c r="D8" t="s">
-        <v>37</v>
-      </c>
       <c r="E8">
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G8">
         <v>190</v>
       </c>
       <c r="H8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E9">
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G9">
         <v>190</v>
       </c>
       <c r="H9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E10">
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G10">
         <v>190</v>
       </c>
       <c r="H10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E11">
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G11">
         <v>190</v>
       </c>
       <c r="H11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E12">
         <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G12">
         <v>190</v>
       </c>
       <c r="H12" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E13">
         <v>10</v>
       </c>
       <c r="F13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G13">
         <v>190</v>
       </c>
       <c r="H13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14">
         <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G14">
         <v>190</v>
       </c>
       <c r="H14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E15">
         <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G15">
         <v>190</v>
       </c>
       <c r="H15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16">
         <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G16">
         <v>190</v>
       </c>
       <c r="H16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E17">
         <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G17">
         <v>190</v>
       </c>
       <c r="H17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E18">
         <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G18">
         <v>190</v>
       </c>
       <c r="H18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E19">
         <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G19">
         <v>190</v>
       </c>
       <c r="H19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E20">
         <v>10</v>
       </c>
       <c r="F20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G20">
         <v>190</v>
       </c>
       <c r="H20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E21">
         <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G21">
         <v>190</v>
       </c>
       <c r="H21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E22">
         <v>10</v>
       </c>
       <c r="F22" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G22">
         <v>190</v>
       </c>
       <c r="H22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E23">
         <v>10</v>
       </c>
       <c r="F23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G23">
         <v>190</v>
       </c>
       <c r="H23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D24" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E24">
         <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G24">
         <v>190</v>
       </c>
       <c r="H24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D25" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E25">
         <v>10</v>
       </c>
       <c r="F25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G25">
         <v>190</v>
       </c>
       <c r="H25" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E26">
         <v>10</v>
       </c>
       <c r="F26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G26">
         <v>190</v>
       </c>
       <c r="H26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D27" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E27">
         <v>10</v>
       </c>
       <c r="F27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G27">
         <v>190</v>
       </c>
       <c r="H27" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D28" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E28">
         <v>10</v>
       </c>
       <c r="F28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G28">
         <v>190</v>
       </c>
       <c r="H28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E29">
         <v>10</v>
       </c>
       <c r="F29" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G29">
         <v>190</v>
       </c>
       <c r="H29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B30" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E30">
         <v>10</v>
       </c>
       <c r="F30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G30">
         <v>190</v>
       </c>
       <c r="H30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E31">
         <v>10</v>
       </c>
       <c r="F31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G31">
         <v>190</v>
       </c>
       <c r="H31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C32" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E32">
         <v>10</v>
       </c>
       <c r="F32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G32">
         <v>190</v>
       </c>
       <c r="H32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B33" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C33" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E33">
         <v>10</v>
       </c>
       <c r="F33" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G33">
         <v>190</v>
       </c>
       <c r="H33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C34" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D34" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E34">
         <v>10</v>
       </c>
       <c r="F34" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G34">
         <v>190</v>
       </c>
       <c r="H34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B35" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C35" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D35" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E35">
         <v>10</v>
       </c>
       <c r="F35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G35">
         <v>190</v>
       </c>
       <c r="H35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B36" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E36">
         <v>10</v>
       </c>
       <c r="F36" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G36">
         <v>190</v>
       </c>
       <c r="H36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B37" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C37" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D37" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E37">
         <v>10</v>
       </c>
       <c r="F37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G37">
         <v>190</v>
       </c>
       <c r="H37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B38" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C38" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E38">
         <v>10</v>
       </c>
       <c r="F38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G38">
         <v>190</v>
       </c>
       <c r="H38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B39" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E39">
         <v>10</v>
       </c>
       <c r="F39" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G39">
         <v>190</v>
       </c>
       <c r="H39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B40" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C40" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E40">
         <v>10</v>
       </c>
       <c r="F40" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G40">
         <v>190</v>
       </c>
       <c r="H40" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>